<commit_message>
GAAp Gl Account added
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/TestCases/MDOT/TC_SM_FOU_DeleteProfile.xlsx
+++ b/src/main/java/TestSuite/MDOT/TestCases/MDOT/TC_SM_FOU_DeleteProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\MDOT\TestCases\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE464F18-7F06-42AB-9655-C5A83C8D28B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4373186-EA3C-4209-A9CC-1C90B08253FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="890" windowWidth="18780" windowHeight="9910" activeTab="1" xr2:uid="{27A31DFA-24AF-4BE1-9FF9-9403A37291B8}"/>
+    <workbookView xWindow="420" yWindow="880" windowWidth="18780" windowHeight="9920" activeTab="1" xr2:uid="{27A31DFA-24AF-4BE1-9FF9-9403A37291B8}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Keyword</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>Enter Text to delete GAAP Category Profile</t>
+  </si>
+  <si>
+    <t>Enter Text to delete GAAP Gl Account Class Profile</t>
   </si>
 </sst>
 </file>
@@ -695,10 +698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155C1548-3305-4173-92A7-939CD1DB0F71}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,6 +792,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>